<commit_message>
Added to doubly linked lists evaluation
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/Doubly Linked Buffer/MPMC_Buffer_Test_Data.xlsx
+++ b/Data Structures/linked_list/Doubly Linked Buffer/MPMC_Buffer_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="113">
   <si>
     <t xml:space="preserve"> Lockless Linked List Key Range 131072 (2^17)</t>
   </si>
@@ -319,6 +319,45 @@
   </si>
   <si>
     <t>Cube (16 Core) 131072 Lockless</t>
+  </si>
+  <si>
+    <t>Compare-and-swap</t>
+  </si>
+  <si>
+    <t>Test-and-set</t>
+  </si>
+  <si>
+    <t>Test-and-test-and-set</t>
+  </si>
+  <si>
+    <t>TAS has a lot more cycles due to its structure but fewer instructions to execute as a result</t>
+  </si>
+  <si>
+    <t>TAS with fewer cache references &amp; a lower proportion of cache misses</t>
+  </si>
+  <si>
+    <t>TTAS uses its cycles quite efficiently</t>
+  </si>
+  <si>
+    <t>Cycles</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Cache References</t>
+  </si>
+  <si>
+    <t>Cache Misses</t>
+  </si>
+  <si>
+    <t>Stalled Frontend Cycles</t>
+  </si>
+  <si>
+    <t>Stalled Backend Cycles</t>
+  </si>
+  <si>
+    <t>Lockless</t>
   </si>
 </sst>
 </file>
@@ -365,7 +404,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -380,6 +419,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -420,7 +461,15 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Doubly Linked Buffer; Stoker; Locked;</a:t>
+              <a:t>Doubly Linked Buffer; Stoker; Compare-and-swap, Test-and-set &amp;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Test-and-test-and-set locks</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>;</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -440,15 +489,15 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$11</c:f>
+              <c:f>Sheet1!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Stoker (32 Core) 128 Locked</c:v>
+                  <c:v>Stoker (32 Core) 128 CAS lock</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -488,33 +537,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$11:$I$11</c:f>
+              <c:f>Sheet1!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>6094274</c:v>
+                  <c:v>5949172</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6093844</c:v>
+                  <c:v>5960837</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3191730</c:v>
+                  <c:v>3123662</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2968884</c:v>
+                  <c:v>3151064</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2290854</c:v>
+                  <c:v>3254280</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1061063</c:v>
+                  <c:v>3260422</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>956667</c:v>
+                  <c:v>3376652</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>927074</c:v>
+                  <c:v>3621271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -522,15 +571,15 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$12</c:f>
+              <c:f>Sheet1!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Stoker (32 Core) 128 CAS lock</c:v>
+                  <c:v>Stoker (32 Core) 128 TAS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -570,88 +619,6 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$I$12</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>5949172</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5960837</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3123662</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3151064</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3254280</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3260422</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3376652</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3621271</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$15</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Stoker (32 Core) 128 TAS</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$B$10:$I$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet1!$B$15:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
@@ -687,7 +654,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
-          <c:order val="3"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
               <c:f>Sheet1!$A$18</c:f>
@@ -777,11 +744,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="44940288"/>
-        <c:axId val="44942464"/>
+        <c:axId val="113076096"/>
+        <c:axId val="113086464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44940288"/>
+        <c:axId val="113076096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -810,7 +777,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44942464"/>
+        <c:crossAx val="113086464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +785,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44942464"/>
+        <c:axId val="113086464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,7 +815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="44940288"/>
+        <c:crossAx val="113076096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1287,11 +1254,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93847552"/>
-        <c:axId val="93849856"/>
+        <c:axId val="113400064"/>
+        <c:axId val="113402624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93847552"/>
+        <c:axId val="113400064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1287,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93849856"/>
+        <c:crossAx val="113402624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1328,7 +1295,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93849856"/>
+        <c:axId val="113402624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1358,7 +1325,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93847552"/>
+        <c:crossAx val="113400064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2289,11 +2256,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="33152384"/>
-        <c:axId val="45320064"/>
+        <c:axId val="113471872"/>
+        <c:axId val="113473792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="33152384"/>
+        <c:axId val="113471872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2322,7 +2289,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="45320064"/>
+        <c:crossAx val="113473792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2330,7 +2297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45320064"/>
+        <c:axId val="113473792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2360,7 +2327,490 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="33152384"/>
+        <c:crossAx val="113471872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-IE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Doubly Linked Buffer; Stoker; Best Performing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Locks vs Lockless</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>;</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 128 Key Range</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 128 CAS lock</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Z$19:$AG$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$20:$AG$20</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5949172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5960837</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3123662</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3151064</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3254280</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3260422</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3376652</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3621271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 128 TAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Z$19:$AG$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$21:$AG$21</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5993999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4848986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6832317</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3919244</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6808247</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6184161</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4102146</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4193558</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 128 TTAS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Z$19:$AG$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$22:$AG$22</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5981033</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5573104</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3754635</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3784453</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3803067</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5744112</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8077373</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4097078</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Y$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Stoker (32 Core) 128 Lockless</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$Z$19:$AG$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Z$23:$AG$23</c:f>
+              <c:numCache>
+                <c:formatCode>_(* #,##0.00_);_(* \(#,##0.00\);_(* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0" formatCode="0.00E+00">
+                  <c:v>4416877</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5423874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6407599</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1523954</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>710103</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>437256</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>537154</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>941193</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="113356160"/>
+        <c:axId val="113478656"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="113356160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113478656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="113478656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Iterations per second</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="113356160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2386,16 +2836,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>990600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>123826</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2418,16 +2868,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1047750</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>476249</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2450,16 +2900,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2475,6 +2925,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2770,10 +3252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A6:O436"/>
+  <dimension ref="A6:AG436"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" topLeftCell="K7" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2786,7 +3268,11 @@
     <col min="7" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="9.140625" customWidth="1"/>
+    <col min="25" max="25" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -3012,7 +3498,7 @@
         <v>37616</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -3041,7 +3527,7 @@
         <v>478154</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -3070,7 +3556,7 @@
         <v>4097078</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -3098,8 +3584,56 @@
       <c r="I19" s="6">
         <v>587783</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>2</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <v>32</v>
+      </c>
+      <c r="S19">
+        <v>64</v>
+      </c>
+      <c r="T19">
+        <v>128</v>
+      </c>
+      <c r="Z19">
+        <v>1</v>
+      </c>
+      <c r="AA19">
+        <v>2</v>
+      </c>
+      <c r="AB19">
+        <v>4</v>
+      </c>
+      <c r="AC19">
+        <v>8</v>
+      </c>
+      <c r="AD19">
+        <v>16</v>
+      </c>
+      <c r="AE19">
+        <v>32</v>
+      </c>
+      <c r="AF19">
+        <v>64</v>
+      </c>
+      <c r="AG19">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>78</v>
       </c>
@@ -3127,8 +3661,62 @@
       <c r="I20" s="6">
         <v>482565</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>70</v>
+      </c>
+      <c r="M20" s="6">
+        <v>5949172</v>
+      </c>
+      <c r="N20" s="6">
+        <v>5960837</v>
+      </c>
+      <c r="O20" s="6">
+        <v>3123662</v>
+      </c>
+      <c r="P20" s="6">
+        <v>3151064</v>
+      </c>
+      <c r="Q20" s="6">
+        <v>3254280</v>
+      </c>
+      <c r="R20" s="6">
+        <v>3260422</v>
+      </c>
+      <c r="S20" s="6">
+        <v>3376652</v>
+      </c>
+      <c r="T20" s="6">
+        <v>3621271</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z20" s="6">
+        <v>5949172</v>
+      </c>
+      <c r="AA20" s="6">
+        <v>5960837</v>
+      </c>
+      <c r="AB20" s="6">
+        <v>3123662</v>
+      </c>
+      <c r="AC20" s="6">
+        <v>3151064</v>
+      </c>
+      <c r="AD20" s="6">
+        <v>3254280</v>
+      </c>
+      <c r="AE20" s="6">
+        <v>3260422</v>
+      </c>
+      <c r="AF20" s="6">
+        <v>3376652</v>
+      </c>
+      <c r="AG20" s="6">
+        <v>3621271</v>
+      </c>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -3156,8 +3744,62 @@
       <c r="I21" s="6">
         <v>2306</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M21" s="6">
+        <v>5993999</v>
+      </c>
+      <c r="N21" s="6">
+        <v>4848986</v>
+      </c>
+      <c r="O21" s="6">
+        <v>6832317</v>
+      </c>
+      <c r="P21" s="6">
+        <v>3919244</v>
+      </c>
+      <c r="Q21" s="6">
+        <v>6808247</v>
+      </c>
+      <c r="R21" s="6">
+        <v>6184161</v>
+      </c>
+      <c r="S21" s="6">
+        <v>4102146</v>
+      </c>
+      <c r="T21" s="6">
+        <v>4193558</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z21" s="6">
+        <v>5993999</v>
+      </c>
+      <c r="AA21" s="6">
+        <v>4848986</v>
+      </c>
+      <c r="AB21" s="6">
+        <v>6832317</v>
+      </c>
+      <c r="AC21" s="6">
+        <v>3919244</v>
+      </c>
+      <c r="AD21" s="6">
+        <v>6808247</v>
+      </c>
+      <c r="AE21" s="6">
+        <v>6184161</v>
+      </c>
+      <c r="AF21" s="6">
+        <v>4102146</v>
+      </c>
+      <c r="AG21" s="6">
+        <v>4193558</v>
+      </c>
+    </row>
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>80</v>
       </c>
@@ -3185,8 +3827,62 @@
       <c r="I22" s="6">
         <v>37151</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>76</v>
+      </c>
+      <c r="M22" s="6">
+        <v>5981033</v>
+      </c>
+      <c r="N22" s="6">
+        <v>5573104</v>
+      </c>
+      <c r="O22" s="6">
+        <v>3754635</v>
+      </c>
+      <c r="P22" s="6">
+        <v>3784453</v>
+      </c>
+      <c r="Q22" s="6">
+        <v>3803067</v>
+      </c>
+      <c r="R22" s="6">
+        <v>5744112</v>
+      </c>
+      <c r="S22" s="6">
+        <v>8077373</v>
+      </c>
+      <c r="T22" s="6">
+        <v>4097078</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z22" s="6">
+        <v>5981033</v>
+      </c>
+      <c r="AA22" s="6">
+        <v>5573104</v>
+      </c>
+      <c r="AB22" s="6">
+        <v>3754635</v>
+      </c>
+      <c r="AC22" s="6">
+        <v>3784453</v>
+      </c>
+      <c r="AD22" s="6">
+        <v>3803067</v>
+      </c>
+      <c r="AE22" s="6">
+        <v>5744112</v>
+      </c>
+      <c r="AF22" s="6">
+        <v>8077373</v>
+      </c>
+      <c r="AG22" s="6">
+        <v>4097078</v>
+      </c>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -3214,8 +3910,35 @@
       <c r="I23" s="6">
         <v>408992</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="Y23" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="Z23" s="11">
+        <v>4416877</v>
+      </c>
+      <c r="AA23" s="7">
+        <v>5423874</v>
+      </c>
+      <c r="AB23" s="7">
+        <v>6407599</v>
+      </c>
+      <c r="AC23" s="7">
+        <v>1523954</v>
+      </c>
+      <c r="AD23" s="7">
+        <v>710103</v>
+      </c>
+      <c r="AE23" s="7">
+        <v>437256</v>
+      </c>
+      <c r="AF23" s="7">
+        <v>537154</v>
+      </c>
+      <c r="AG23" s="7">
+        <v>941193</v>
+      </c>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -3243,8 +3966,35 @@
       <c r="I24" s="6">
         <v>13963807</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>17</v>
+      </c>
+      <c r="M24" s="10">
+        <v>85308079089</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P24" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q24" s="10">
+        <v>83654891182</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="T24" t="s">
+        <v>25</v>
+      </c>
+      <c r="U24" s="10">
+        <v>2720105582388</v>
+      </c>
+      <c r="V24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -3272,8 +4022,35 @@
       <c r="I25" s="6">
         <v>8690874</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M25" s="10">
+        <v>79994895074</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q25" s="10">
+        <v>86505423537</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="U25" s="10">
+        <v>35474162702</v>
+      </c>
+      <c r="V25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y25" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z25" s="10">
+        <v>1901831500205</v>
+      </c>
+      <c r="AA25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3301,8 +4078,33 @@
       <c r="I26" s="6">
         <v>1107</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M26" s="10">
+        <v>86035699</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q26" s="10">
+        <v>111460201</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="U26" s="10">
+        <v>354385343</v>
+      </c>
+      <c r="V26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y26" s="4"/>
+      <c r="Z26" s="10">
+        <v>134361208960</v>
+      </c>
+      <c r="AA26" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -3330,8 +4132,42 @@
       <c r="I27" s="6">
         <v>6401511</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M27" s="10">
+        <v>77068971</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O27">
+        <v>89.577898355890611</v>
+      </c>
+      <c r="Q27" s="10">
+        <v>102277723</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="S27">
+        <v>91.761653112396587</v>
+      </c>
+      <c r="U27" s="10">
+        <v>285703484</v>
+      </c>
+      <c r="V27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="W27">
+        <v>80.619441419731629</v>
+      </c>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="10">
+        <v>670122662</v>
+      </c>
+      <c r="AA27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -3359,8 +4195,37 @@
       <c r="I28" s="6">
         <v>3570434</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M28" s="10">
+        <v>15791646425</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q28" s="10">
+        <v>17434765060</v>
+      </c>
+      <c r="R28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U28" s="10">
+        <v>7816648547</v>
+      </c>
+      <c r="V28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="10">
+        <v>417186847</v>
+      </c>
+      <c r="AA28" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB28">
+        <f>Z28/Z27*100</f>
+        <v>62.255296031161535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -3388,8 +4253,41 @@
       <c r="I29" s="6">
         <v>3859491</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M29" s="10">
+        <v>3857290</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O29">
+        <v>2.4426142127229142E-2</v>
+      </c>
+      <c r="Q29" s="10">
+        <v>5733887</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S29">
+        <v>3.2887664274611109E-2</v>
+      </c>
+      <c r="U29" s="10">
+        <v>16485489</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W29">
+        <v>0.2109022671401424</v>
+      </c>
+      <c r="Z29" s="10">
+        <v>43911916506</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -3417,8 +4315,36 @@
       <c r="I30" s="6">
         <v>48043</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M30" s="10">
+        <v>7497711279</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q30" s="10">
+        <v>7512907878</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U30" s="10">
+        <v>172802362385</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z30" s="10">
+        <v>53412889</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB30">
+        <f>Z30/Z29*100</f>
+        <v>0.12163643322810065</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -3446,8 +4372,32 @@
       <c r="I31" s="6">
         <v>4506048</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M31" s="10">
+        <v>56870.871408999999</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="10">
+        <v>57050.815692999997</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="U31" s="10">
+        <v>1306160.0975959999</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z31" s="10">
+        <v>131573431168</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -3475,8 +4425,32 @@
       <c r="I32" s="6">
         <v>8333710</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M32" s="10">
+        <v>56871.115091</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="10">
+        <v>57050.967133999999</v>
+      </c>
+      <c r="R32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U32" s="10">
+        <v>1306157.0382419999</v>
+      </c>
+      <c r="V32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z32" s="10">
+        <v>997297.92553899996</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -3504,8 +4478,41 @@
       <c r="I33" s="6">
         <v>2327420</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M33" s="10">
+        <v>52355183299</v>
+      </c>
+      <c r="N33" t="s">
+        <v>13</v>
+      </c>
+      <c r="O33">
+        <v>61.371893328390406</v>
+      </c>
+      <c r="Q33" s="10">
+        <v>48079634126</v>
+      </c>
+      <c r="R33" t="s">
+        <v>13</v>
+      </c>
+      <c r="S33">
+        <v>57.473787182865024</v>
+      </c>
+      <c r="U33" s="10">
+        <v>2702865287076</v>
+      </c>
+      <c r="V33" t="s">
+        <v>13</v>
+      </c>
+      <c r="W33">
+        <v>99.366190216158273</v>
+      </c>
+      <c r="Z33" s="10">
+        <v>997267.49901200004</v>
+      </c>
+      <c r="AA33" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -3533,8 +4540,45 @@
       <c r="I34" s="6">
         <v>3421791</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M34" s="10">
+        <v>41366005089</v>
+      </c>
+      <c r="N34" t="s">
+        <v>14</v>
+      </c>
+      <c r="O34">
+        <v>48.49013778149169</v>
+      </c>
+      <c r="Q34" s="10">
+        <v>39626617921</v>
+      </c>
+      <c r="R34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S34">
+        <v>47.369158409145655</v>
+      </c>
+      <c r="U34" s="10">
+        <v>2634229355419</v>
+      </c>
+      <c r="V34" t="s">
+        <v>14</v>
+      </c>
+      <c r="W34">
+        <v>96.842908322197971</v>
+      </c>
+      <c r="Z34" s="10">
+        <v>1825851385993</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB34">
+        <f>Z34/Z25*100</f>
+        <v>96.004897689211163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -3562,8 +4606,21 @@
       <c r="I35" s="6">
         <v>1951927</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="Z35" s="10">
+        <v>1539810715708</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB35">
+        <f>Z35/Z25*100</f>
+        <v>80.964623603196316</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -3591,8 +4648,26 @@
       <c r="I36" s="6">
         <v>4180428</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>106</v>
+      </c>
+      <c r="N36" t="s">
+        <v>107</v>
+      </c>
+      <c r="O36" t="s">
+        <v>108</v>
+      </c>
+      <c r="P36" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>110</v>
+      </c>
+      <c r="R36" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -3620,8 +4695,29 @@
       <c r="I37" s="6">
         <v>4053571</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L37" t="s">
+        <v>100</v>
+      </c>
+      <c r="M37" s="10">
+        <v>83654891182</v>
+      </c>
+      <c r="N37" s="10">
+        <v>86505423537</v>
+      </c>
+      <c r="O37" s="10">
+        <v>111460201</v>
+      </c>
+      <c r="P37" s="10">
+        <v>102277723</v>
+      </c>
+      <c r="Q37" s="10">
+        <v>48079634126</v>
+      </c>
+      <c r="R37" s="10">
+        <v>39626617921</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -3649,8 +4745,29 @@
       <c r="I38" s="7">
         <v>233</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L38" t="s">
+        <v>101</v>
+      </c>
+      <c r="M38" s="10">
+        <v>2720105582388</v>
+      </c>
+      <c r="N38" s="10">
+        <v>35474162702</v>
+      </c>
+      <c r="O38" s="10">
+        <v>354385343</v>
+      </c>
+      <c r="P38" s="10">
+        <v>285703484</v>
+      </c>
+      <c r="Q38" s="10">
+        <v>2702865287076</v>
+      </c>
+      <c r="R38" s="10">
+        <v>2634229355419</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -3678,8 +4795,29 @@
       <c r="I39" s="6">
         <v>6485220</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L39" t="s">
+        <v>102</v>
+      </c>
+      <c r="M39" s="10">
+        <v>85308079089</v>
+      </c>
+      <c r="N39" s="10">
+        <v>79994895074</v>
+      </c>
+      <c r="O39" s="10">
+        <v>86035699</v>
+      </c>
+      <c r="P39" s="10">
+        <v>77068971</v>
+      </c>
+      <c r="Q39" s="10">
+        <v>52355183299</v>
+      </c>
+      <c r="R39" s="10">
+        <v>41366005089</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -3707,8 +4845,29 @@
       <c r="I40" s="6">
         <v>120213</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L40" t="s">
+        <v>112</v>
+      </c>
+      <c r="M40">
+        <v>1901831500205</v>
+      </c>
+      <c r="N40">
+        <v>134361208960</v>
+      </c>
+      <c r="O40" s="1">
+        <v>670122662</v>
+      </c>
+      <c r="P40" s="1">
+        <v>417186847</v>
+      </c>
+      <c r="Q40">
+        <v>1825851385993</v>
+      </c>
+      <c r="R40" s="1">
+        <v>1539810715708</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -3736,8 +4895,11 @@
       <c r="I41" s="6">
         <v>313834</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -3765,8 +4927,11 @@
       <c r="I42" s="6">
         <v>5411589</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>62</v>
       </c>
@@ -3794,8 +4959,11 @@
       <c r="I43" s="6">
         <v>1040529</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L43" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>63</v>
       </c>
@@ -3824,7 +4992,7 @@
         <v>4330903</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>64</v>
       </c>
@@ -3853,7 +5021,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -3882,7 +5050,7 @@
         <v>111106</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>67</v>
       </c>
@@ -3895,7 +5063,7 @@
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="B49">
         <v>1</v>
       </c>
@@ -3921,7 +5089,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -3950,7 +5118,7 @@
         <v>949825</v>
       </c>
     </row>
-    <row r="51" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -3978,8 +5146,20 @@
       <c r="I51" s="6">
         <v>3910836</v>
       </c>
-    </row>
-    <row r="52" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+    </row>
+    <row r="52" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -4008,7 +5188,7 @@
         <v>558429</v>
       </c>
     </row>
-    <row r="53" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -4037,7 +5217,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -4065,8 +5245,20 @@
       <c r="I54" s="6">
         <v>4382517</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3"/>
+      <c r="T54" s="3"/>
+      <c r="U54" s="3"/>
+      <c r="V54" s="3"/>
+      <c r="W54" s="3"/>
+    </row>
+    <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -4095,7 +5287,7 @@
         <v>38184</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -4123,9 +5315,8 @@
       <c r="I56" s="6">
         <v>485102</v>
       </c>
-      <c r="L56" s="1"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -4153,8 +5344,9 @@
       <c r="I57" s="6">
         <v>3471701</v>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L57" s="1"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -4183,7 +5375,7 @@
         <v>582545</v>
       </c>
     </row>
-    <row r="59" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -4211,8 +5403,20 @@
       <c r="I59" s="6">
         <v>480256</v>
       </c>
-    </row>
-    <row r="60" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+      <c r="O59"/>
+      <c r="P59"/>
+      <c r="Q59"/>
+      <c r="R59"/>
+      <c r="S59"/>
+      <c r="T59"/>
+      <c r="U59"/>
+      <c r="V59"/>
+      <c r="W59"/>
+    </row>
+    <row r="60" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -4240,9 +5444,8 @@
       <c r="I60" s="6">
         <v>2386</v>
       </c>
-      <c r="L60" s="5"/>
-    </row>
-    <row r="61" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -4272,7 +5475,7 @@
       </c>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>42</v>
       </c>
@@ -4284,9 +5487,20 @@
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
-      <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L62" s="5"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="3"/>
+      <c r="U62" s="3"/>
+      <c r="V62" s="3"/>
+      <c r="W62" s="3"/>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -4300,7 +5514,7 @@
       <c r="I63" s="6"/>
       <c r="L63" s="1"/>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>44</v>
       </c>
@@ -4313,9 +5527,8 @@
       <c r="H64" s="6"/>
       <c r="I64" s="6"/>
       <c r="L64" s="1"/>
-      <c r="O64" s="2"/>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>45</v>
       </c>
@@ -4330,7 +5543,7 @@
       <c r="L65" s="1"/>
       <c r="O65" s="2"/>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>46</v>
       </c>
@@ -4342,8 +5555,10 @@
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
       <c r="I66" s="6"/>
-    </row>
-    <row r="67" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L66" s="1"/>
+      <c r="O66" s="2"/>
+    </row>
+    <row r="67" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -4355,9 +5570,20 @@
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
       <c r="I67" s="6"/>
-      <c r="L67" s="5"/>
-    </row>
-    <row r="68" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+    </row>
+    <row r="68" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>48</v>
       </c>
@@ -4369,8 +5595,9 @@
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
       <c r="I68" s="6"/>
-    </row>
-    <row r="69" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L68" s="5"/>
+    </row>
+    <row r="69" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>49</v>
       </c>
@@ -4382,9 +5609,8 @@
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
-      <c r="L69" s="5"/>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>50</v>
       </c>
@@ -4396,10 +5622,20 @@
       <c r="G70" s="6"/>
       <c r="H70" s="6"/>
       <c r="I70" s="6"/>
-      <c r="L70" s="1"/>
-      <c r="O70" s="2"/>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L70" s="5"/>
+      <c r="M70" s="3"/>
+      <c r="N70" s="3"/>
+      <c r="O70" s="3"/>
+      <c r="P70" s="3"/>
+      <c r="Q70" s="3"/>
+      <c r="R70" s="3"/>
+      <c r="S70" s="3"/>
+      <c r="T70" s="3"/>
+      <c r="U70" s="3"/>
+      <c r="V70" s="3"/>
+      <c r="W70" s="3"/>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>51</v>
       </c>
@@ -4414,7 +5650,7 @@
       <c r="L71" s="1"/>
       <c r="O71" s="2"/>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>52</v>
       </c>
@@ -4429,7 +5665,7 @@
       <c r="L72" s="1"/>
       <c r="O72" s="2"/>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>53</v>
       </c>
@@ -4444,7 +5680,7 @@
       <c r="L73" s="1"/>
       <c r="O73" s="2"/>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>54</v>
       </c>
@@ -4456,8 +5692,10 @@
       <c r="G74" s="6"/>
       <c r="H74" s="6"/>
       <c r="I74" s="6"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L74" s="1"/>
+      <c r="O74" s="2"/>
+    </row>
+    <row r="75" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>55</v>
       </c>
@@ -4470,7 +5708,7 @@
       <c r="H75" s="6"/>
       <c r="I75" s="6"/>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>56</v>
       </c>
@@ -4483,7 +5721,7 @@
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>57</v>
       </c>
@@ -4495,9 +5733,8 @@
       <c r="G77" s="7"/>
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
-      <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>58</v>
       </c>
@@ -4511,7 +5748,7 @@
       <c r="I78" s="6"/>
       <c r="L78" s="1"/>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>59</v>
       </c>
@@ -4525,7 +5762,7 @@
       <c r="I79" s="6"/>
       <c r="L79" s="1"/>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>60</v>
       </c>
@@ -4552,7 +5789,6 @@
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
       <c r="L81" s="1"/>
-      <c r="O81" s="2"/>
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -4582,6 +5818,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
       <c r="L83" s="1"/>
+      <c r="O83" s="2"/>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -4595,6 +5832,7 @@
       <c r="G84" s="6"/>
       <c r="H84" s="6"/>
       <c r="I84" s="6"/>
+      <c r="L84" s="1"/>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
@@ -4608,11 +5846,9 @@
       <c r="G85" s="6"/>
       <c r="H85" s="6"/>
       <c r="I85" s="6"/>
-      <c r="L85" s="1"/>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L86" s="1"/>
-      <c r="O86" s="2"/>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
@@ -4626,6 +5862,8 @@
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
       <c r="I87" s="9"/>
+      <c r="L87" s="1"/>
+      <c r="O87" s="2"/>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B88">
@@ -4739,7 +5977,6 @@
       <c r="I91" s="7">
         <v>5855952</v>
       </c>
-      <c r="L91" s="1"/>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
@@ -4749,7 +5986,6 @@
       <c r="A93" s="4"/>
       <c r="B93" s="1"/>
       <c r="L93" s="1"/>
-      <c r="O93" s="2"/>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
@@ -4769,6 +6005,7 @@
       <c r="H95" s="9"/>
       <c r="I95" s="9"/>
       <c r="L95" s="1"/>
+      <c r="O95" s="2"/>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B96">
@@ -4795,6 +6032,7 @@
       <c r="I96">
         <v>128</v>
       </c>
+      <c r="L96" s="1"/>
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
@@ -4824,7 +6062,6 @@
       <c r="I97" s="7">
         <v>1677683</v>
       </c>
-      <c r="L97" s="1"/>
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
@@ -4839,7 +6076,6 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="L98" s="1"/>
-      <c r="O98" s="2"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
@@ -4853,6 +6089,8 @@
       <c r="G99" s="7"/>
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
+      <c r="L99" s="1"/>
+      <c r="O99" s="2"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
@@ -4868,7 +6106,6 @@
       <c r="A102" s="4"/>
       <c r="B102" s="1"/>
       <c r="E102" s="2"/>
-      <c r="L102" s="1"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
@@ -4882,6 +6119,7 @@
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
       <c r="I103" s="9"/>
+      <c r="L103" s="1"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B104">
@@ -4908,7 +6146,6 @@
       <c r="I104">
         <v>128</v>
       </c>
-      <c r="L104" s="1"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
@@ -4937,7 +6174,6 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="L106" s="1"/>
-      <c r="O106" s="2"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
@@ -4957,20 +6193,20 @@
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="L108" s="1"/>
+      <c r="O108" s="2"/>
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
+      <c r="L109" s="1"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L110" s="1"/>
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="L111" s="1"/>
-      <c r="O111" s="2"/>
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
@@ -4991,6 +6227,8 @@
       <c r="G112" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="L112" s="1"/>
+      <c r="O112" s="2"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
@@ -5080,7 +6318,6 @@
         <f>F117/F116*100</f>
         <v>0.14910606307756591</v>
       </c>
-      <c r="L117" s="1"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B118" s="1">
@@ -5113,7 +6350,6 @@
         <v>10</v>
       </c>
       <c r="L119" s="1"/>
-      <c r="O119" s="2"/>
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B120" s="1">
@@ -5155,6 +6391,7 @@
       </c>
       <c r="J121" s="8"/>
       <c r="L121" s="1"/>
+      <c r="O121" s="2"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B122" s="1">
@@ -5178,6 +6415,7 @@
         <v>50.799918030948511</v>
       </c>
       <c r="J122" s="8"/>
+      <c r="L122" s="1"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B123" s="1"/>
@@ -5185,17 +6423,17 @@
       <c r="E123" s="2"/>
       <c r="F123" s="6"/>
       <c r="J123" s="8"/>
-      <c r="L123" s="1"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C124" s="1"/>
       <c r="F124" s="2"/>
       <c r="J124" s="8"/>
       <c r="L124" s="1"/>
-      <c r="O124" s="2"/>
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J125" s="8"/>
+      <c r="L125" s="1"/>
+      <c r="O125" s="2"/>
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.25">
       <c r="J126" s="8"/>

</xml_diff>